<commit_message>
added new feature Page Setup the key AutoSize(true,false(default)) Also completed the writing of an excel file based on a Visio diagram.   Note at this time the connections to shapes are disabled.
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectDataBlueprinting.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectDataBlueprinting.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70571EFF-312A-4FF4-AB7B-ADC1A9D9F561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897C30B-6F60-470E-8C9D-2240C3485CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="690" windowWidth="23910" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24930" yWindow="915" windowWidth="22200" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Doug Vidakovich</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A3856540-2A7D-4F32-9DAA-D6863B596B4B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{23F258D9-1ECF-47DA-8B2F-3F0B88B29C2C}">
       <text>
         <r>
           <rPr>
@@ -60,11 +60,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+if the first character is ';' this line will be ignored. This is concidered a comment.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2C58DBFA-D082-43D3-9A8C-B1F609470680}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{AF6E03B1-8AF6-454C-AEB4-442370390D4B}">
       <text>
         <r>
           <rPr>
@@ -91,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{78C66964-03C3-4C36-BD13-79480B7AFFBF}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{89A89032-B67E-4AA5-957E-7DE4C065E1CB}">
       <text>
         <r>
           <rPr>
@@ -114,7 +115,18 @@
           <t xml:space="preserve">
 the ShapeImage value must be first and exactly the same as the ShapeImage value.
 Followed by ':' character
-followed by a unique value which makes this value unique to all other ShapeKey values</t>
+followed by a unique value which makes this value unique to all other ShapeKey values
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>easy was to set this field is use the stencil name + ':' + row value</t>
         </r>
         <r>
           <rPr>
@@ -128,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{623C1581-E966-4EB4-9B66-7D6FEE18CCF7}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D35BEA42-F808-4BD7-A828-07911C0D01EE}">
       <text>
         <r>
           <rPr>
@@ -154,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A71CAD57-4F41-4F15-AF0C-1230FC9CC194}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{22984143-7D8C-4A0C-803E-3C096D1BD9AC}">
       <text>
         <r>
           <rPr>
@@ -220,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="351">
   <si>
     <t>Shape</t>
   </si>
@@ -766,9 +778,6 @@
   </si>
   <si>
     <t>Shape Type</t>
-  </si>
-  <si>
-    <t>Shape Key</t>
   </si>
   <si>
     <t>Shape Image</t>
@@ -1068,9 +1077,6 @@
     <t>;Integrations</t>
   </si>
   <si>
-    <t>TableCell</t>
-  </si>
-  <si>
     <t>TableCell:R1C1</t>
   </si>
   <si>
@@ -1134,9 +1140,6 @@
     <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
   </si>
   <si>
-    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Advocate_CustomStencils.vssx</t>
-  </si>
-  <si>
     <t>Line Pattern</t>
   </si>
   <si>
@@ -1249,6 +1252,78 @@
   </si>
   <si>
     <t>;0</t>
+  </si>
+  <si>
+    <t>Unique Key</t>
+  </si>
+  <si>
+    <t>Shape Label Font Size</t>
+  </si>
+  <si>
+    <t>C:\Omnicell\Projects\AdvocateAurora\Data\Stencils\Advocate_CustomStencils.vssx</t>
+  </si>
+  <si>
+    <t>OC_Logo</t>
+  </si>
+  <si>
+    <t>OC_Footer</t>
+  </si>
+  <si>
+    <t>OC_Group4</t>
+  </si>
+  <si>
+    <t>OC_Server</t>
+  </si>
+  <si>
+    <t>OC_IconKey2</t>
+  </si>
+  <si>
+    <t>OC_LineLedgen</t>
+  </si>
+  <si>
+    <t>OC_Ethernet2</t>
+  </si>
+  <si>
+    <t>OC_PortsLDAP_info</t>
+  </si>
+  <si>
+    <t>OC_DashOutline</t>
+  </si>
+  <si>
+    <t>OC_DB</t>
+  </si>
+  <si>
+    <t>OC_OISInterfaces</t>
+  </si>
+  <si>
+    <t>OC_Title</t>
+  </si>
+  <si>
+    <t>OC_Group2</t>
+  </si>
+  <si>
+    <t>OC_BlisterPackager</t>
+  </si>
+  <si>
+    <t>OC_CPM</t>
+  </si>
+  <si>
+    <t>OC_YuyamaPackager</t>
+  </si>
+  <si>
+    <t>OC_Carousel</t>
+  </si>
+  <si>
+    <t>OC_XR2</t>
+  </si>
+  <si>
+    <t>OC_AIO</t>
+  </si>
+  <si>
+    <t>OC_TagLabeler</t>
+  </si>
+  <si>
+    <t>OC_TableCell</t>
   </si>
 </sst>
 </file>
@@ -2423,11 +2498,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,7 +2511,7 @@
     <col min="1" max="1" width="24.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" style="2" hidden="1" customWidth="1"/>
@@ -2467,46 +2543,46 @@
   <sheetData>
     <row r="1" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>176</v>
       </c>
       <c r="C1" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="E1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>180</v>
+        <v>328</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>17</v>
@@ -2515,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R1" s="50" t="s">
         <v>12</v>
@@ -2530,42 +2606,42 @@
         <v>15</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AB1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AC1" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>191</v>
-      </c>
-      <c r="AF1" s="34" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -2601,17 +2677,17 @@
     </row>
     <row r="3" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -2654,14 +2730,14 @@
         <v>0</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -2704,14 +2780,14 @@
         <v>0</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>291</v>
+        <v>329</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -2751,7 +2827,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2796,7 +2872,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
@@ -2843,22 +2919,22 @@
         <v>0</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
@@ -2902,10 +2978,10 @@
         <v>59</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>3</v>
+        <v>331</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F9" s="21">
         <v>9</v>
@@ -2992,7 +3068,7 @@
         <v>97</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>32</v>
@@ -3044,7 +3120,7 @@
         <v>98</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>99</v>
@@ -3074,7 +3150,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="W12" s="21"/>
       <c r="X12" s="23"/>
@@ -3086,7 +3162,7 @@
       </c>
       <c r="AC12" s="23"/>
       <c r="AD12" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE12" s="19" t="s">
         <v>27</v>
@@ -3106,7 +3182,7 @@
         <v>95</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>47</v>
@@ -3136,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="W13" s="21"/>
       <c r="X13" s="23"/>
@@ -3148,7 +3224,7 @@
       </c>
       <c r="AC13" s="23"/>
       <c r="AD13" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE13" s="19" t="s">
         <v>27</v>
@@ -3168,7 +3244,7 @@
         <v>94</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>49</v>
@@ -3198,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="W14" s="21" t="s">
         <v>58</v>
@@ -3207,7 +3283,7 @@
         <v>46</v>
       </c>
       <c r="Y14" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z14" s="23" t="s">
         <v>30</v>
@@ -3220,7 +3296,7 @@
       </c>
       <c r="AC14" s="23"/>
       <c r="AD14" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE14" s="19" t="s">
         <v>27</v>
@@ -3240,7 +3316,7 @@
         <v>96</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>48</v>
@@ -3270,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="W15" s="21"/>
       <c r="X15" s="23"/>
@@ -3282,7 +3358,7 @@
       </c>
       <c r="AC15" s="23"/>
       <c r="AD15" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE15" s="19" t="s">
         <v>27</v>
@@ -3302,7 +3378,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>93</v>
@@ -3332,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="W16" s="23" t="s">
         <v>58</v>
@@ -3341,7 +3417,7 @@
         <v>55</v>
       </c>
       <c r="Y16" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z16" s="23" t="s">
         <v>29</v>
@@ -3356,7 +3432,7 @@
         <v>56</v>
       </c>
       <c r="AD16" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE16" s="23" t="s">
         <v>30</v>
@@ -3372,7 +3448,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -3414,7 +3490,7 @@
         <v>92</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>89</v>
+        <v>334</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -3464,7 +3540,7 @@
         <v>63</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>41</v>
@@ -3518,7 +3594,7 @@
         <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>42</v>
@@ -3572,7 +3648,7 @@
         <v>65</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>43</v>
@@ -3626,7 +3702,7 @@
         <v>66</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>34</v>
+        <v>335</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>35</v>
@@ -3680,7 +3756,7 @@
         <v>67</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>34</v>
+        <v>335</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>36</v>
@@ -3734,10 +3810,10 @@
         <v>68</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>34</v>
+        <v>335</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -3784,7 +3860,7 @@
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -3826,10 +3902,10 @@
         <v>58</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>40</v>
+        <v>336</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -3867,7 +3943,7 @@
       <c r="AE26" s="19"/>
       <c r="AF26" s="23"/>
     </row>
-    <row r="27" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>1</v>
       </c>
@@ -3878,7 +3954,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>4</v>
+        <v>337</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
@@ -3964,7 +4040,7 @@
         <v>79</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>44</v>
@@ -4003,7 +4079,7 @@
       </c>
       <c r="X29" s="23"/>
       <c r="Y29" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z29" s="23" t="s">
         <v>27</v>
@@ -4018,7 +4094,7 @@
         <v>53</v>
       </c>
       <c r="AD29" s="23" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AE29" s="23" t="s">
         <v>30</v>
@@ -4038,7 +4114,7 @@
         <v>80</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>45</v>
@@ -4077,7 +4153,7 @@
       </c>
       <c r="X30" s="23"/>
       <c r="Y30" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z30" s="23" t="s">
         <v>27</v>
@@ -4099,13 +4175,13 @@
         <v>0</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>172</v>
@@ -4192,10 +4268,10 @@
         <v>169</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>172</v>
@@ -4246,7 +4322,7 @@
         <v>81</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>173</v>
@@ -4285,7 +4361,7 @@
       </c>
       <c r="X34" s="23"/>
       <c r="Y34" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z34" s="23" t="s">
         <v>27</v>
@@ -4310,10 +4386,10 @@
         <v>82</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>18</v>
+        <v>339</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -4350,7 +4426,7 @@
       </c>
       <c r="AC35" s="23"/>
       <c r="AD35" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE35" s="23" t="s">
         <v>27</v>
@@ -4370,10 +4446,10 @@
         <v>83</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>18</v>
+        <v>339</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
@@ -4410,7 +4486,7 @@
       </c>
       <c r="AC36" s="23"/>
       <c r="AD36" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE36" s="23" t="s">
         <v>27</v>
@@ -4430,7 +4506,7 @@
         <v>84</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>174</v>
@@ -4469,7 +4545,7 @@
       </c>
       <c r="X37" s="23"/>
       <c r="Y37" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z37" s="23" t="s">
         <v>27</v>
@@ -4482,7 +4558,7 @@
       </c>
       <c r="AC37" s="23"/>
       <c r="AD37" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE37" s="23" t="s">
         <v>27</v>
@@ -4502,7 +4578,7 @@
         <v>91</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>11</v>
+        <v>340</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
@@ -4540,7 +4616,7 @@
       </c>
       <c r="AC38" s="23"/>
       <c r="AD38" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE38" s="23" t="s">
         <v>27</v>
@@ -4593,13 +4669,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>172</v>
@@ -4650,10 +4726,10 @@
         <v>85</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
@@ -4689,7 +4765,7 @@
       </c>
       <c r="X41" s="23"/>
       <c r="Y41" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z41" s="23" t="s">
         <v>27</v>
@@ -4714,10 +4790,10 @@
         <v>86</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>50</v>
+        <v>333</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
@@ -4753,7 +4829,7 @@
       </c>
       <c r="X42" s="23"/>
       <c r="Y42" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z42" s="23" t="s">
         <v>27</v>
@@ -4766,7 +4842,7 @@
       </c>
       <c r="AC42" s="23"/>
       <c r="AD42" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE42" s="23" t="s">
         <v>27</v>
@@ -4786,7 +4862,7 @@
         <v>90</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>11</v>
+        <v>340</v>
       </c>
       <c r="E43" s="21" t="s">
         <v>51</v>
@@ -4826,7 +4902,7 @@
       </c>
       <c r="AC43" s="23"/>
       <c r="AD43" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE43" s="23" t="s">
         <v>27</v>
@@ -4882,7 +4958,7 @@
         <v>125</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
@@ -4932,10 +5008,10 @@
         <v>126</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>2</v>
+        <v>341</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
@@ -4984,10 +5060,10 @@
         <v>127</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>3</v>
+        <v>331</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F47" s="32">
         <v>10</v>
@@ -5074,7 +5150,7 @@
         <v>88</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>87</v>
+        <v>342</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>154</v>
@@ -5126,10 +5202,10 @@
         <v>130</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>40</v>
+        <v>336</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
@@ -5214,7 +5290,7 @@
         <v>75</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>5</v>
+        <v>343</v>
       </c>
       <c r="E52" s="17" t="s">
         <v>115</v>
@@ -5254,7 +5330,7 @@
       </c>
       <c r="AC52" s="19"/>
       <c r="AD52" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE52" s="19" t="s">
         <v>28</v>
@@ -5272,7 +5348,7 @@
         <v>76</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E53" s="17" t="s">
         <v>116</v>
@@ -5312,7 +5388,7 @@
       </c>
       <c r="AC53" s="19"/>
       <c r="AD53" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE53" s="19" t="s">
         <v>28</v>
@@ -5330,7 +5406,7 @@
         <v>77</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>5</v>
+        <v>343</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>117</v>
@@ -5370,7 +5446,7 @@
       </c>
       <c r="AC54" s="27"/>
       <c r="AD54" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE54" s="27" t="s">
         <v>28</v>
@@ -5388,7 +5464,7 @@
         <v>78</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>118</v>
@@ -5428,7 +5504,7 @@
       </c>
       <c r="AC55" s="27"/>
       <c r="AD55" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE55" s="27" t="s">
         <v>28</v>
@@ -5446,7 +5522,7 @@
         <v>73</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>6</v>
+        <v>345</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>114</v>
@@ -5486,7 +5562,7 @@
       </c>
       <c r="AC56" s="19"/>
       <c r="AD56" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE56" s="19" t="s">
         <v>28</v>
@@ -5504,7 +5580,7 @@
         <v>74</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>119</v>
@@ -5544,7 +5620,7 @@
       </c>
       <c r="AC57" s="19"/>
       <c r="AD57" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE57" s="19" t="s">
         <v>28</v>
@@ -5562,7 +5638,7 @@
         <v>71</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>120</v>
@@ -5602,7 +5678,7 @@
       </c>
       <c r="AC58" s="27"/>
       <c r="AD58" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE58" s="27" t="s">
         <v>28</v>
@@ -5620,7 +5696,7 @@
         <v>105</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E59" s="28" t="s">
         <v>112</v>
@@ -5660,7 +5736,7 @@
       </c>
       <c r="AC59" s="27"/>
       <c r="AD59" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE59" s="27" t="s">
         <v>28</v>
@@ -5678,7 +5754,7 @@
         <v>72</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>121</v>
@@ -5718,7 +5794,7 @@
       </c>
       <c r="AC60" s="19"/>
       <c r="AD60" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE60" s="19" t="s">
         <v>28</v>
@@ -5736,7 +5812,7 @@
         <v>106</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E61" s="17" t="s">
         <v>111</v>
@@ -5776,7 +5852,7 @@
       </c>
       <c r="AC61" s="19"/>
       <c r="AD61" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE61" s="19" t="s">
         <v>28</v>
@@ -5794,7 +5870,7 @@
         <v>101</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E62" s="28" t="s">
         <v>122</v>
@@ -5834,7 +5910,7 @@
       </c>
       <c r="AC62" s="27"/>
       <c r="AD62" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE62" s="27" t="s">
         <v>28</v>
@@ -5852,7 +5928,7 @@
         <v>103</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>110</v>
@@ -5892,7 +5968,7 @@
       </c>
       <c r="AC63" s="27"/>
       <c r="AD63" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE63" s="27" t="s">
         <v>28</v>
@@ -5910,10 +5986,10 @@
         <v>102</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
@@ -5950,7 +6026,7 @@
       </c>
       <c r="AC64" s="19"/>
       <c r="AD64" s="19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AE64" s="19" t="s">
         <v>28</v>
@@ -5970,10 +6046,10 @@
         <v>104</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
@@ -6010,7 +6086,7 @@
       </c>
       <c r="AC65" s="19"/>
       <c r="AD65" s="19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AE65" s="19" t="s">
         <v>28</v>
@@ -6027,13 +6103,13 @@
         <v>0</v>
       </c>
       <c r="C66" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E66" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="E66" s="21" t="s">
-        <v>225</v>
       </c>
       <c r="F66" s="21"/>
       <c r="G66" s="21"/>
@@ -6084,7 +6160,7 @@
         <v>69</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="E67" s="28" t="s">
         <v>8</v>
@@ -6124,7 +6200,7 @@
       </c>
       <c r="AC67" s="27"/>
       <c r="AD67" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE67" s="27" t="s">
         <v>28</v>
@@ -6142,7 +6218,7 @@
         <v>107</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>124</v>
@@ -6182,7 +6258,7 @@
       </c>
       <c r="AC68" s="27"/>
       <c r="AD68" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE68" s="27" t="s">
         <v>28</v>
@@ -6200,7 +6276,7 @@
         <v>70</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>33</v>
@@ -6240,7 +6316,7 @@
       </c>
       <c r="AC69" s="19"/>
       <c r="AD69" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE69" s="19" t="s">
         <v>28</v>
@@ -6258,7 +6334,7 @@
         <v>108</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>123</v>
@@ -6298,7 +6374,7 @@
       </c>
       <c r="AC70" s="19"/>
       <c r="AD70" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE70" s="19" t="s">
         <v>28</v>
@@ -6316,7 +6392,7 @@
         <v>100</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E71" s="28" t="s">
         <v>113</v>
@@ -6356,7 +6432,7 @@
       </c>
       <c r="AC71" s="27"/>
       <c r="AD71" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE71" s="27" t="s">
         <v>27</v>
@@ -6410,7 +6486,7 @@
         <v>158</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>109</v>
+        <v>348</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>159</v>
@@ -6450,7 +6526,7 @@
       </c>
       <c r="AC73" s="19"/>
       <c r="AD73" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE73" s="19" t="s">
         <v>28</v>
@@ -6468,7 +6544,7 @@
         <v>168</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>156</v>
+        <v>349</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>167</v>
@@ -6508,7 +6584,7 @@
       </c>
       <c r="AC74" s="19"/>
       <c r="AD74" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE74" s="19" t="s">
         <v>28</v>
@@ -6562,7 +6638,7 @@
         <v>131</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>87</v>
+        <v>342</v>
       </c>
       <c r="E76" s="21" t="s">
         <v>155</v>
@@ -6614,7 +6690,7 @@
         <v>132</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>4</v>
+        <v>337</v>
       </c>
       <c r="E77" s="21"/>
       <c r="F77" s="21"/>
@@ -6700,7 +6776,7 @@
         <v>134</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>5</v>
+        <v>343</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>115</v>
@@ -6740,7 +6816,7 @@
       </c>
       <c r="AC79" s="19"/>
       <c r="AD79" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE79" s="19" t="s">
         <v>28</v>
@@ -6758,7 +6834,7 @@
         <v>133</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E80" s="17" t="s">
         <v>116</v>
@@ -6798,7 +6874,7 @@
       </c>
       <c r="AC80" s="19"/>
       <c r="AD80" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE80" s="19" t="s">
         <v>28</v>
@@ -6816,7 +6892,7 @@
         <v>152</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>5</v>
+        <v>343</v>
       </c>
       <c r="E81" s="28" t="s">
         <v>117</v>
@@ -6856,7 +6932,7 @@
       </c>
       <c r="AC81" s="27"/>
       <c r="AD81" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE81" s="27" t="s">
         <v>28</v>
@@ -6874,7 +6950,7 @@
         <v>135</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E82" s="28" t="s">
         <v>118</v>
@@ -6914,7 +6990,7 @@
       </c>
       <c r="AC82" s="27"/>
       <c r="AD82" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE82" s="27" t="s">
         <v>28</v>
@@ -6932,7 +7008,7 @@
         <v>136</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>6</v>
+        <v>345</v>
       </c>
       <c r="E83" s="17" t="s">
         <v>153</v>
@@ -6972,7 +7048,7 @@
       </c>
       <c r="AC83" s="19"/>
       <c r="AD83" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE83" s="19" t="s">
         <v>28</v>
@@ -6990,7 +7066,7 @@
         <v>137</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E84" s="17" t="s">
         <v>119</v>
@@ -7030,7 +7106,7 @@
       </c>
       <c r="AC84" s="19"/>
       <c r="AD84" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE84" s="19" t="s">
         <v>28</v>
@@ -7048,7 +7124,7 @@
         <v>138</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E85" s="28" t="s">
         <v>120</v>
@@ -7088,7 +7164,7 @@
       </c>
       <c r="AC85" s="27"/>
       <c r="AD85" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE85" s="27" t="s">
         <v>28</v>
@@ -7106,7 +7182,7 @@
         <v>139</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E86" s="28" t="s">
         <v>112</v>
@@ -7146,7 +7222,7 @@
       </c>
       <c r="AC86" s="27"/>
       <c r="AD86" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE86" s="27" t="s">
         <v>28</v>
@@ -7164,7 +7240,7 @@
         <v>140</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>121</v>
@@ -7204,7 +7280,7 @@
       </c>
       <c r="AC87" s="19"/>
       <c r="AD87" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE87" s="19" t="s">
         <v>28</v>
@@ -7222,7 +7298,7 @@
         <v>142</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E88" s="17" t="s">
         <v>111</v>
@@ -7262,7 +7338,7 @@
       </c>
       <c r="AC88" s="19"/>
       <c r="AD88" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE88" s="19" t="s">
         <v>28</v>
@@ -7280,7 +7356,7 @@
         <v>143</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E89" s="28" t="s">
         <v>122</v>
@@ -7320,7 +7396,7 @@
       </c>
       <c r="AC89" s="27"/>
       <c r="AD89" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE89" s="27" t="s">
         <v>28</v>
@@ -7338,7 +7414,7 @@
         <v>144</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E90" s="28" t="s">
         <v>110</v>
@@ -7378,7 +7454,7 @@
       </c>
       <c r="AC90" s="27"/>
       <c r="AD90" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE90" s="27" t="s">
         <v>28</v>
@@ -7396,10 +7472,10 @@
         <v>145</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="17"/>
@@ -7436,7 +7512,7 @@
       </c>
       <c r="AC91" s="19"/>
       <c r="AD91" s="19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AE91" s="19" t="s">
         <v>28</v>
@@ -7456,10 +7532,10 @@
         <v>146</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="17"/>
@@ -7496,7 +7572,7 @@
       </c>
       <c r="AC92" s="19"/>
       <c r="AD92" s="19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AE92" s="19" t="s">
         <v>28</v>
@@ -7513,13 +7589,13 @@
         <v>0</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="E93" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F93" s="21"/>
       <c r="G93" s="21"/>
@@ -7570,7 +7646,7 @@
         <v>147</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="E94" s="28" t="s">
         <v>8</v>
@@ -7610,7 +7686,7 @@
       </c>
       <c r="AC94" s="27"/>
       <c r="AD94" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE94" s="27" t="s">
         <v>28</v>
@@ -7628,7 +7704,7 @@
         <v>148</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E95" s="28" t="s">
         <v>124</v>
@@ -7668,7 +7744,7 @@
       </c>
       <c r="AC95" s="27"/>
       <c r="AD95" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE95" s="27" t="s">
         <v>28</v>
@@ -7686,7 +7762,7 @@
         <v>149</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>33</v>
@@ -7726,7 +7802,7 @@
       </c>
       <c r="AC96" s="19"/>
       <c r="AD96" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE96" s="19" t="s">
         <v>28</v>
@@ -7744,7 +7820,7 @@
         <v>150</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E97" s="17" t="s">
         <v>123</v>
@@ -7784,7 +7860,7 @@
       </c>
       <c r="AC97" s="19"/>
       <c r="AD97" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE97" s="19" t="s">
         <v>28</v>
@@ -7802,7 +7878,7 @@
         <v>151</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>10</v>
+        <v>344</v>
       </c>
       <c r="E98" s="28" t="s">
         <v>129</v>
@@ -7842,7 +7918,7 @@
       </c>
       <c r="AC98" s="27"/>
       <c r="AD98" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE98" s="27" t="s">
         <v>27</v>
@@ -7896,7 +7972,7 @@
         <v>141</v>
       </c>
       <c r="D100" s="17" t="s">
-        <v>109</v>
+        <v>348</v>
       </c>
       <c r="E100" s="17" t="s">
         <v>157</v>
@@ -7936,7 +8012,7 @@
       </c>
       <c r="AC100" s="19"/>
       <c r="AD100" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE100" s="19" t="s">
         <v>28</v>
@@ -7954,7 +8030,7 @@
         <v>166</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>156</v>
+        <v>349</v>
       </c>
       <c r="E101" s="17" t="s">
         <v>167</v>
@@ -7994,7 +8070,7 @@
       </c>
       <c r="AC101" s="19"/>
       <c r="AD101" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE101" s="19" t="s">
         <v>28</v>
@@ -8048,7 +8124,7 @@
         <v>171</v>
       </c>
       <c r="D103" s="21" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E103" s="32" t="s">
         <v>175</v>
@@ -8090,7 +8166,7 @@
       </c>
       <c r="AC103" s="23"/>
       <c r="AD103" s="19" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AE103" s="19" t="s">
         <v>27</v>
@@ -8101,7 +8177,7 @@
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
@@ -8143,13 +8219,13 @@
         <v>0</v>
       </c>
       <c r="C105" s="40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E105" s="41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F105" s="41">
         <v>8</v>
@@ -8199,13 +8275,13 @@
         <v>0</v>
       </c>
       <c r="C106" s="40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E106" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F106" s="41">
         <v>8</v>
@@ -8255,13 +8331,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="40" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E107" s="41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F107" s="41">
         <v>8</v>
@@ -8311,13 +8387,13 @@
         <v>0</v>
       </c>
       <c r="C108" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E108" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F108" s="32">
         <v>8</v>
@@ -8365,13 +8441,13 @@
         <v>0</v>
       </c>
       <c r="C109" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D109" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E109" s="32" t="s">
         <v>274</v>
-      </c>
-      <c r="D109" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="E109" s="32" t="s">
-        <v>276</v>
       </c>
       <c r="F109" s="32">
         <v>8</v>
@@ -8419,13 +8495,13 @@
         <v>0</v>
       </c>
       <c r="C110" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="D110" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E110" s="32" t="s">
         <v>275</v>
-      </c>
-      <c r="D110" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="E110" s="32" t="s">
-        <v>277</v>
       </c>
       <c r="F110" s="32">
         <v>8</v>
@@ -8473,13 +8549,13 @@
         <v>0</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E111" s="41" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F111" s="41">
         <v>8</v>
@@ -8508,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="V111" s="43" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="W111" s="40"/>
       <c r="X111" s="39"/>
@@ -8529,13 +8605,13 @@
         <v>0</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E112" s="41" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F112" s="41">
         <v>8</v>
@@ -8564,7 +8640,7 @@
         <v>0</v>
       </c>
       <c r="V112" s="43" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="W112" s="40"/>
       <c r="X112" s="39"/>
@@ -8585,10 +8661,10 @@
         <v>0</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>269</v>
+        <v>350</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>48</v>
@@ -8620,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="V113" s="43" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="W113" s="40"/>
       <c r="X113" s="39"/>
@@ -8639,7 +8715,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5EA153F9-C5B8-4862-A9CE-AB94CB69D12A}">
           <x14:formula1>
             <xm:f>Tables!#REF!</xm:f>
@@ -8670,12 +8746,6 @@
           </x14:formula1>
           <xm:sqref>Y2:Y113 AD2:AD113</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{000CBC19-A464-4694-A3AD-9D82A1CE6A27}">
-          <x14:formula1>
-            <xm:f>Tables!$I$2:$I$49</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D113</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -8684,6 +8754,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F0DF1A-7900-47BA-8B9D-42C3E7E31390}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8701,7 +8772,7 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
@@ -8727,13 +8798,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
       <c r="F4" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58"/>
@@ -8748,49 +8819,49 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B5" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>237</v>
-      </c>
       <c r="F5" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H5" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="J5" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="K5" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="L5" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="M5" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="M5" s="38" t="s">
+      <c r="N5" s="38" t="s">
         <v>244</v>
-      </c>
-      <c r="N5" s="38" t="s">
-        <v>245</v>
       </c>
       <c r="O5" s="38" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -8859,7 +8930,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="F9" s="59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G9" s="60"/>
       <c r="H9" s="60"/>
@@ -8877,7 +8948,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10" s="65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G10" s="60"/>
       <c r="H10" s="60"/>
@@ -8886,7 +8957,7 @@
       <c r="K10" s="60"/>
       <c r="L10" s="60"/>
       <c r="M10" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N10" s="63"/>
       <c r="O10" s="64"/>
@@ -8896,7 +8967,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F11" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
@@ -8929,6 +9000,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E06A7CC-7A58-4BCC-B48C-DB107FF0CF1F}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A3:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8944,69 +9016,69 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="66"/>
       <c r="C3" s="66"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="C4" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="37" t="s">
         <v>260</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -9022,6 +9094,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0736EE8-23D0-4513-9563-3C6A65BAEEB4}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9038,7 +9111,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="39" t="s">
@@ -9046,14 +9119,14 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="45" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9074,7 +9147,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I3" s="47" t="s">
         <v>109</v>
@@ -9088,13 +9161,13 @@
         <v>29</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9108,7 +9181,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I5" s="47" t="s">
         <v>5</v>
@@ -9116,16 +9189,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I6" s="47" t="s">
         <v>7</v>
@@ -9139,7 +9212,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -9147,7 +9220,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I8" s="47" t="s">
         <v>10</v>
@@ -9155,13 +9228,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E9" s="16">
         <v>10</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -9172,7 +9245,7 @@
         <v>172</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -9183,7 +9256,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="47" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -9191,7 +9264,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I12" s="47" t="s">
         <v>18</v>
@@ -9199,21 +9272,21 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E13" s="16">
         <v>12</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -9221,12 +9294,12 @@
         <v>14</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I16" s="51" t="s">
         <v>3</v>
@@ -9234,7 +9307,7 @@
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="47" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
@@ -9244,17 +9317,17 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="47" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="47" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="47" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
@@ -9264,12 +9337,12 @@
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="47" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="47" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
@@ -9284,7 +9357,7 @@
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="47" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
@@ -9294,22 +9367,22 @@
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="51" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="47" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="47" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
@@ -9319,7 +9392,7 @@
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="47" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
@@ -9334,27 +9407,27 @@
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="47" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="47" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="47" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="47" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="47" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
@@ -9369,12 +9442,12 @@
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" s="47" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="47" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.25">
@@ -9384,7 +9457,7 @@
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I47" s="47" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.25">
@@ -9394,7 +9467,7 @@
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="52" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>